<commit_message>
Made field name as fieldName and property name as PropertyName.
</commit_message>
<xml_diff>
--- a/Example/Excel/Example.xlsx
+++ b/Example/Excel/Example.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Documents\Unity\QuickSheet\Assets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28125"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680"/>
+    <workbookView xWindow="980" yWindow="420" windowWidth="24280" windowHeight="14240"/>
   </bookViews>
   <sheets>
     <sheet name="ExcelExample" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>Id</t>
   </si>
@@ -75,17 +73,43 @@
   </si>
   <si>
     <t>Lurker</t>
+  </si>
+  <si>
+    <t>Strength Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -107,14 +131,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="5">
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -172,7 +204,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -224,7 +256,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -418,7 +450,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -426,15 +458,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,8 +482,11 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>0</v>
       </c>
@@ -461,8 +499,11 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -475,8 +516,11 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>2</v>
       </c>
@@ -489,8 +533,11 @@
       <c r="D4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>3</v>
       </c>
@@ -503,8 +550,11 @@
       <c r="D5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>4</v>
       </c>
@@ -517,8 +567,11 @@
       <c r="D6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>5</v>
       </c>
@@ -531,8 +584,11 @@
       <c r="D7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>6</v>
       </c>
@@ -545,8 +601,11 @@
       <c r="D8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>7</v>
       </c>
@@ -559,8 +618,11 @@
       <c r="D9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>8</v>
       </c>
@@ -573,8 +635,11 @@
       <c r="D10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>9</v>
       </c>
@@ -587,8 +652,18 @@
       <c r="D11" t="s">
         <v>5</v>
       </c>
+      <c r="E11">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>